<commit_message>
additional data and update readme
</commit_message>
<xml_diff>
--- a/raw_data/album_info_metadata_neutral.xlsx
+++ b/raw_data/album_info_metadata_neutral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aucklandmuseum-my.sharepoint.com/personal/mklemm_aucklandmuseum_com/Documents/Documents/Personal/FunAnalysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aucklandmuseum-my.sharepoint.com/personal/mklemm_aucklandmuseum_com/Documents/Documents/Personal/ScreamingColor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1683" documentId="11_B99231273CA9E3883874B2AD939D86AFF492890B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8703B5B0-AC36-40A9-8150-108EEE54576F}"/>
+  <xr:revisionPtr revIDLastSave="1689" documentId="11_B99231273CA9E3883874B2AD939D86AFF492890B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86F3A19D-0A06-4696-800F-DCAF39184BB3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -3411,9 +3411,6 @@
     <t>regretful</t>
   </si>
   <si>
-    <t>breakup, regretful, hearbreak</t>
-  </si>
-  <si>
     <t>You always regretful what you don't say</t>
   </si>
   <si>
@@ -3573,9 +3570,6 @@
     <t>equality</t>
   </si>
   <si>
-    <t>LGBT+ rights, protest, politics, bullying</t>
-  </si>
-  <si>
     <t>vulnerability</t>
   </si>
   <si>
@@ -4504,6 +4498,12 @@
   </si>
   <si>
     <t>neutral; negative;neutral; neutral; negative</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>breakup, regretful, heartbreak</t>
   </si>
 </sst>
 </file>
@@ -5032,7 +5032,7 @@
   <dimension ref="A1:AN242"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5104,19 +5104,19 @@
         <v>751</v>
       </c>
       <c r="I1" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="J1" t="s">
         <v>752</v>
       </c>
       <c r="K1" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="L1" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="M1" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="N1" t="s">
         <v>753</v>
@@ -5223,23 +5223,23 @@
         <v>874</v>
       </c>
       <c r="H2" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="I2">
-        <f>LEN(H2)-LEN(SUBSTITUTE(H2, ",", ""))+1</f>
+        <f t="shared" ref="I2:I65" si="0">LEN(H2)-LEN(SUBSTITUTE(H2, ",", ""))+1</f>
         <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="K2" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="L2" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M2" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
@@ -5330,23 +5330,23 @@
         <v>1058</v>
       </c>
       <c r="G3" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="H3" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="I3">
-        <f>LEN(H3)-LEN(SUBSTITUTE(H3, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="L3" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M3" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="P3" t="s">
         <v>30</v>
@@ -5440,23 +5440,23 @@
         <v>1058</v>
       </c>
       <c r="G4" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="H4" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="I4">
-        <f>LEN(H4)-LEN(SUBSTITUTE(H4, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="L4" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M4" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="P4" t="s">
         <v>30</v>
@@ -5553,23 +5553,23 @@
         <v>778</v>
       </c>
       <c r="H5" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="I5">
-        <f>LEN(H5)-LEN(SUBSTITUTE(H5, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J5" t="s">
         <v>1102</v>
       </c>
       <c r="K5" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="L5" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M5" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="P5" t="s">
         <v>30</v>
@@ -5663,26 +5663,26 @@
         <v>1037</v>
       </c>
       <c r="H6" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="I6">
-        <f>LEN(H6)-LEN(SUBSTITUTE(H6, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J6" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="K6" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="L6" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M6" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
       <c r="N6" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="P6" t="s">
         <v>30</v>
@@ -5778,23 +5778,23 @@
         <v>778</v>
       </c>
       <c r="H7" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="I7">
-        <f>LEN(H7)-LEN(SUBSTITUTE(H7, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J7" t="s">
         <v>1102</v>
       </c>
       <c r="K7" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="L7" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M7" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="P7" t="s">
         <v>30</v>
@@ -5885,23 +5885,23 @@
         <v>765</v>
       </c>
       <c r="G8" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H8" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="I8">
-        <f>LEN(H8)-LEN(SUBSTITUTE(H8, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="L8" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="M8" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="P8" t="s">
         <v>30</v>
@@ -5998,17 +5998,17 @@
         <v>887</v>
       </c>
       <c r="I9">
-        <f>LEN(H9)-LEN(SUBSTITUTE(H9, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K9" t="s">
         <v>1004</v>
       </c>
       <c r="L9" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="M9" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="P9" t="s">
         <v>30</v>
@@ -6105,7 +6105,7 @@
         <v>1050</v>
       </c>
       <c r="I10">
-        <f>LEN(H10)-LEN(SUBSTITUTE(H10, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J10" t="s">
@@ -6115,10 +6115,10 @@
         <v>1051</v>
       </c>
       <c r="L10" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M10" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="O10" t="s">
         <v>963</v>
@@ -6215,10 +6215,10 @@
         <v>1111</v>
       </c>
       <c r="H11" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="I11">
-        <f>LEN(H11)-LEN(SUBSTITUTE(H11, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J11" t="s">
@@ -6228,10 +6228,10 @@
         <v>1115</v>
       </c>
       <c r="L11" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="M11" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="P11" t="s">
         <v>30</v>
@@ -6324,13 +6324,13 @@
         <v>1124</v>
       </c>
       <c r="G12" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H12" t="s">
         <v>1137</v>
       </c>
-      <c r="H12" t="s">
-        <v>1138</v>
-      </c>
       <c r="I12">
-        <f>LEN(H12)-LEN(SUBSTITUTE(H12, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J12" t="s">
@@ -6340,10 +6340,10 @@
         <v>1119</v>
       </c>
       <c r="L12" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="M12" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="P12" t="s">
         <v>30</v>
@@ -6436,23 +6436,23 @@
         <v>882</v>
       </c>
       <c r="G13" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="H13" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="I13">
-        <f>LEN(H13)-LEN(SUBSTITUTE(H13, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="L13" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M13" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="P13" t="s">
         <v>30</v>
@@ -6546,23 +6546,23 @@
         <v>869</v>
       </c>
       <c r="H14" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="I14">
-        <f>LEN(H14)-LEN(SUBSTITUTE(H14, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J14" t="s">
         <v>30</v>
       </c>
       <c r="K14" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="L14" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M14" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="P14" t="s">
         <v>30</v>
@@ -6656,23 +6656,23 @@
         <v>869</v>
       </c>
       <c r="H15" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="I15">
-        <f>LEN(H15)-LEN(SUBSTITUTE(H15, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J15" t="s">
         <v>30</v>
       </c>
       <c r="K15" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="L15" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M15" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="P15" t="s">
         <v>30</v>
@@ -6715,23 +6715,23 @@
         <v>796</v>
       </c>
       <c r="H16" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="I16">
-        <f>LEN(H16)-LEN(SUBSTITUTE(H16, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J16" t="s">
         <v>1108</v>
       </c>
       <c r="K16" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="L16" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M16" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P16" t="s">
         <v>30</v>
@@ -6830,7 +6830,7 @@
         <v>1064</v>
       </c>
       <c r="I17">
-        <f>LEN(H17)-LEN(SUBSTITUTE(H17, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J17" t="s">
@@ -6840,10 +6840,10 @@
         <v>1086</v>
       </c>
       <c r="L17" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M17" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="O17" t="s">
         <v>970</v>
@@ -6942,20 +6942,20 @@
         <v>806</v>
       </c>
       <c r="H18" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="I18">
-        <f>LEN(H18)-LEN(SUBSTITUTE(H18, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="L18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M18" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P18" t="s">
         <v>30</v>
@@ -7043,29 +7043,29 @@
         <v>687</v>
       </c>
       <c r="F19" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="G19" t="s">
         <v>796</v>
       </c>
       <c r="H19" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="I19">
-        <f>LEN(H19)-LEN(SUBSTITUTE(H19, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J19" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K19" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="L19" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M19" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P19" t="s">
         <v>30</v>
@@ -7156,26 +7156,26 @@
         <v>786</v>
       </c>
       <c r="G20" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H20" t="s">
         <v>1165</v>
       </c>
-      <c r="H20" t="s">
-        <v>1166</v>
-      </c>
       <c r="I20">
-        <f>LEN(H20)-LEN(SUBSTITUTE(H20, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J20" t="s">
         <v>1102</v>
       </c>
       <c r="K20" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="L20" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M20" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
@@ -7266,26 +7266,26 @@
         <v>846</v>
       </c>
       <c r="G21" t="s">
+        <v>1152</v>
+      </c>
+      <c r="H21" t="s">
         <v>1153</v>
       </c>
-      <c r="H21" t="s">
-        <v>1154</v>
-      </c>
       <c r="I21">
-        <f>LEN(H21)-LEN(SUBSTITUTE(H21, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J21" t="s">
         <v>1102</v>
       </c>
       <c r="K21" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="L21" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M21" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P21" t="s">
         <v>30</v>
@@ -7384,17 +7384,17 @@
         <v>779</v>
       </c>
       <c r="I22">
-        <f>LEN(H22)-LEN(SUBSTITUTE(H22, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K22" t="s">
         <v>989</v>
       </c>
       <c r="L22" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M22" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="O22" t="s">
         <v>901</v>
@@ -7491,23 +7491,23 @@
         <v>1024</v>
       </c>
       <c r="H23" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="I23">
-        <f>LEN(H23)-LEN(SUBSTITUTE(H23, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J23" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="K23" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="L23" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M23" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="P23" t="s">
         <v>30</v>
@@ -7604,7 +7604,7 @@
         <v>854</v>
       </c>
       <c r="I24">
-        <f>LEN(H24)-LEN(SUBSTITUTE(H24, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J24" t="s">
@@ -7614,10 +7614,10 @@
         <v>1001</v>
       </c>
       <c r="L24" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M24" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="O24" t="s">
         <v>934</v>
@@ -7685,7 +7685,7 @@
         <v>89</v>
       </c>
       <c r="AM24" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="AN24" t="s">
         <v>197</v>
@@ -7717,17 +7717,17 @@
         <v>774</v>
       </c>
       <c r="I25">
-        <f>LEN(H25)-LEN(SUBSTITUTE(H25, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K25" t="s">
         <v>987</v>
       </c>
       <c r="L25" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="M25" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="O25" t="s">
         <v>899</v>
@@ -7829,7 +7829,7 @@
         <v>888</v>
       </c>
       <c r="I26">
-        <f>LEN(H26)-LEN(SUBSTITUTE(H26, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J26" t="s">
@@ -7839,10 +7839,10 @@
         <v>1005</v>
       </c>
       <c r="L26" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="M26" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="O26" t="s">
         <v>944</v>
@@ -7942,7 +7942,7 @@
         <v>888</v>
       </c>
       <c r="I27">
-        <f>LEN(H27)-LEN(SUBSTITUTE(H27, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J27" t="s">
@@ -7952,10 +7952,10 @@
         <v>1005</v>
       </c>
       <c r="L27" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="M27" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="P27" t="s">
         <v>30</v>
@@ -8049,23 +8049,23 @@
         <v>894</v>
       </c>
       <c r="H28" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="I28">
-        <f>LEN(H28)-LEN(SUBSTITUTE(H28, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J28" t="s">
         <v>1102</v>
       </c>
       <c r="K28" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="L28" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="M28" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="P28" t="s">
         <v>30</v>
@@ -8162,7 +8162,7 @@
         <v>836</v>
       </c>
       <c r="I29">
-        <f>LEN(H29)-LEN(SUBSTITUTE(H29, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J29" t="s">
@@ -8172,10 +8172,10 @@
         <v>1006</v>
       </c>
       <c r="L29" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="M29" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="O29" t="s">
         <v>945</v>
@@ -8243,7 +8243,7 @@
         <v>213</v>
       </c>
       <c r="AM29" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="AN29" t="s">
         <v>253</v>
@@ -8275,7 +8275,7 @@
         <v>1019</v>
       </c>
       <c r="I30">
-        <f>LEN(H30)-LEN(SUBSTITUTE(H30, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J30" t="s">
@@ -8285,10 +8285,10 @@
         <v>1021</v>
       </c>
       <c r="L30" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="M30" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="P30" t="s">
         <v>30</v>
@@ -8379,26 +8379,26 @@
         <v>1124</v>
       </c>
       <c r="G31" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="H31" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="I31">
-        <f>LEN(H31)-LEN(SUBSTITUTE(H31, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J31" t="s">
         <v>1102</v>
       </c>
       <c r="K31" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="L31" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M31" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="P31" t="s">
         <v>30</v>
@@ -8492,23 +8492,23 @@
         <v>755</v>
       </c>
       <c r="H32" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="I32">
-        <f>LEN(H32)-LEN(SUBSTITUTE(H32, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J32" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="K32" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="L32" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M32" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="P32" t="s">
         <v>30</v>
@@ -8605,7 +8605,7 @@
         <v>983</v>
       </c>
       <c r="I33">
-        <f>LEN(H33)-LEN(SUBSTITUTE(H33, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J33" t="s">
@@ -8615,10 +8615,10 @@
         <v>986</v>
       </c>
       <c r="L33" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M33" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="O33" t="s">
         <v>958</v>
@@ -8715,23 +8715,23 @@
         <v>834</v>
       </c>
       <c r="H34" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="I34">
-        <f>LEN(H34)-LEN(SUBSTITUTE(H34, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J34" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="K34" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="L34" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="M34" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="P34" t="s">
         <v>30</v>
@@ -8822,26 +8822,26 @@
         <v>775</v>
       </c>
       <c r="G35" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="H35" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I35">
-        <f>LEN(H35)-LEN(SUBSTITUTE(H35, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J35" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="K35" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="L35" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="M35" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="P35" t="s">
         <v>30</v>
@@ -8938,17 +8938,17 @@
         <v>1043</v>
       </c>
       <c r="I36">
-        <f>LEN(H36)-LEN(SUBSTITUTE(H36, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K36" t="s">
         <v>1044</v>
       </c>
       <c r="L36" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M36" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="O36" t="s">
         <v>961</v>
@@ -9042,26 +9042,26 @@
         <v>882</v>
       </c>
       <c r="G37" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="H37" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="I37">
-        <f>LEN(H37)-LEN(SUBSTITUTE(H37, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J37" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="K37" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="L37" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="M37" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="P37" t="s">
         <v>30</v>
@@ -9158,17 +9158,17 @@
         <v>1099</v>
       </c>
       <c r="I38">
-        <f>LEN(H38)-LEN(SUBSTITUTE(H38, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K38" t="s">
         <v>1097</v>
       </c>
       <c r="L38" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M38" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="P38" t="s">
         <v>30</v>
@@ -9208,23 +9208,23 @@
         <v>770</v>
       </c>
       <c r="G39" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="H39" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="I39">
-        <f>LEN(H39)-LEN(SUBSTITUTE(H39, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K39" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="L39" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M39" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="P39" t="s">
         <v>30</v>
@@ -9315,29 +9315,29 @@
         <v>802</v>
       </c>
       <c r="G40" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="H40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="I40">
-        <f>LEN(H40)-LEN(SUBSTITUTE(H40, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J40" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="K40" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="L40" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M40" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="N40" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="P40" t="s">
         <v>30</v>
@@ -9434,7 +9434,7 @@
         <v>1105</v>
       </c>
       <c r="I41">
-        <f>LEN(H41)-LEN(SUBSTITUTE(H41, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J41" t="s">
@@ -9444,10 +9444,10 @@
         <v>1114</v>
       </c>
       <c r="L41" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M41" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="P41" t="s">
         <v>30</v>
@@ -9512,7 +9512,7 @@
         <v>417</v>
       </c>
       <c r="AM41" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="AN41" t="s">
         <v>418</v>
@@ -9544,7 +9544,7 @@
         <v>831</v>
       </c>
       <c r="I42">
-        <f>LEN(H42)-LEN(SUBSTITUTE(H42, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J42" t="s">
@@ -9554,10 +9554,10 @@
         <v>996</v>
       </c>
       <c r="L42" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M42" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="N42" t="s">
         <v>830</v>
@@ -9648,16 +9648,16 @@
         <v>441</v>
       </c>
       <c r="F43" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G43" t="s">
         <v>796</v>
       </c>
       <c r="H43" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="I43">
-        <f>LEN(H43)-LEN(SUBSTITUTE(H43, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J43" t="s">
@@ -9667,10 +9667,10 @@
         <v>1120</v>
       </c>
       <c r="L43" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M43" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="P43" t="s">
         <v>30</v>
@@ -9767,17 +9767,17 @@
         <v>878</v>
       </c>
       <c r="I44">
-        <f>LEN(H44)-LEN(SUBSTITUTE(H44, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K44" t="s">
         <v>1002</v>
       </c>
       <c r="L44" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M44" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="P44" t="s">
         <v>30</v>
@@ -9871,20 +9871,20 @@
         <v>1017</v>
       </c>
       <c r="H45" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="I45">
-        <f>LEN(H45)-LEN(SUBSTITUTE(H45, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K45" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="L45" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M45" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="P45" t="s">
         <v>30</v>
@@ -9981,7 +9981,7 @@
         <v>1074</v>
       </c>
       <c r="I46">
-        <f>LEN(H46)-LEN(SUBSTITUTE(H46, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J46" t="s">
@@ -9991,10 +9991,10 @@
         <v>1091</v>
       </c>
       <c r="L46" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="M46" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="P46" t="s">
         <v>30</v>
@@ -10061,7 +10061,7 @@
         <v>62</v>
       </c>
       <c r="AM46" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="AN46" t="s">
         <v>388</v>
@@ -10090,20 +10090,20 @@
         <v>775</v>
       </c>
       <c r="H47" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="I47">
-        <f>LEN(H47)-LEN(SUBSTITUTE(H47, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K47" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="L47" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="M47" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="P47" t="s">
         <v>30</v>
@@ -10205,7 +10205,7 @@
         <v>1122</v>
       </c>
       <c r="I48">
-        <f>LEN(H48)-LEN(SUBSTITUTE(H48, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J48" t="s">
@@ -10215,10 +10215,10 @@
         <v>1117</v>
       </c>
       <c r="L48" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="M48" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="P48" t="s">
         <v>30</v>
@@ -10315,7 +10315,7 @@
         <v>1104</v>
       </c>
       <c r="I49">
-        <f>LEN(H49)-LEN(SUBSTITUTE(H49, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J49" t="s">
@@ -10325,10 +10325,10 @@
         <v>1113</v>
       </c>
       <c r="L49" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M49" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="P49" t="s">
         <v>30</v>
@@ -10424,23 +10424,23 @@
         <v>846</v>
       </c>
       <c r="G50" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="H50" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="I50">
-        <f>LEN(H50)-LEN(SUBSTITUTE(H50, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K50" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="L50" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
       <c r="M50" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="P50" t="s">
         <v>30</v>
@@ -10537,7 +10537,7 @@
         <v>816</v>
       </c>
       <c r="I51">
-        <f>LEN(H51)-LEN(SUBSTITUTE(H51, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J51" t="s">
@@ -10547,10 +10547,10 @@
         <v>998</v>
       </c>
       <c r="L51" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="M51" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="N51" t="s">
         <v>814</v>
@@ -10653,7 +10653,7 @@
         <v>783</v>
       </c>
       <c r="I52">
-        <f>LEN(H52)-LEN(SUBSTITUTE(H52, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="J52" t="s">
@@ -10663,10 +10663,10 @@
         <v>991</v>
       </c>
       <c r="L52" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M52" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="N52" t="s">
         <v>757</v>
@@ -10763,26 +10763,26 @@
         <v>855</v>
       </c>
       <c r="G53" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="H53" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="I53">
-        <f>LEN(H53)-LEN(SUBSTITUTE(H53, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J53" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K53" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="L53" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M53" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="P53" t="s">
         <v>30</v>
@@ -10876,20 +10876,20 @@
         <v>855</v>
       </c>
       <c r="H54" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="I54">
-        <f>LEN(H54)-LEN(SUBSTITUTE(H54, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K54" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="L54" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M54" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="P54" t="s">
         <v>30</v>
@@ -10983,10 +10983,10 @@
         <v>1100</v>
       </c>
       <c r="H55" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="I55">
-        <f>LEN(H55)-LEN(SUBSTITUTE(H55, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J55" t="s">
@@ -10996,10 +10996,10 @@
         <v>1121</v>
       </c>
       <c r="L55" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="M55" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="P55" t="s">
         <v>30</v>
@@ -11096,17 +11096,17 @@
         <v>883</v>
       </c>
       <c r="I56">
-        <f>LEN(H56)-LEN(SUBSTITUTE(H56, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K56" t="s">
         <v>1003</v>
       </c>
       <c r="L56" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M56" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="P56" t="s">
         <v>30</v>
@@ -11174,7 +11174,7 @@
         <v>39</v>
       </c>
       <c r="AM56" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="AN56" t="s">
         <v>242</v>
@@ -11200,26 +11200,26 @@
         <v>1009</v>
       </c>
       <c r="G57" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H57" t="s">
         <v>1283</v>
       </c>
-      <c r="H57" t="s">
-        <v>1285</v>
-      </c>
       <c r="I57">
-        <f>LEN(H57)-LEN(SUBSTITUTE(H57, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J57" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="K57" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="L57" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M57" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="P57" t="s">
         <v>30</v>
@@ -11319,17 +11319,17 @@
         <v>843</v>
       </c>
       <c r="I58">
-        <f>LEN(H58)-LEN(SUBSTITUTE(H58, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K58" t="s">
         <v>997</v>
       </c>
       <c r="L58" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M58" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="P58" t="s">
         <v>30</v>
@@ -11423,20 +11423,20 @@
         <v>755</v>
       </c>
       <c r="H59" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="I59">
-        <f>LEN(H59)-LEN(SUBSTITUTE(H59, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K59" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="L59" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M59" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="P59" t="s">
         <v>30</v>
@@ -11535,17 +11535,17 @@
         <v>800</v>
       </c>
       <c r="I60">
-        <f>LEN(H60)-LEN(SUBSTITUTE(H60, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K60" t="s">
         <v>990</v>
       </c>
       <c r="L60" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M60" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="O60" t="s">
         <v>902</v>
@@ -11642,23 +11642,23 @@
         <v>796</v>
       </c>
       <c r="H61" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="I61">
-        <f>LEN(H61)-LEN(SUBSTITUTE(H61, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J61" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="K61" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="L61" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="M61" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="P61" t="s">
         <v>30</v>
@@ -11752,23 +11752,23 @@
         <v>882</v>
       </c>
       <c r="H62" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="I62">
-        <f>LEN(H62)-LEN(SUBSTITUTE(H62, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="J62" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K62" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="L62" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M62" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="P62" t="s">
         <v>30</v>
@@ -11862,20 +11862,20 @@
         <v>842</v>
       </c>
       <c r="H63" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="I63">
-        <f>LEN(H63)-LEN(SUBSTITUTE(H63, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="K63" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
       <c r="L63" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M63" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="P63" t="s">
         <v>30</v>
@@ -11972,7 +11972,7 @@
         <v>1069</v>
       </c>
       <c r="I64">
-        <f>LEN(H64)-LEN(SUBSTITUTE(H64, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="J64" t="s">
@@ -11982,10 +11982,10 @@
         <v>1089</v>
       </c>
       <c r="L64" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M64" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="P64" t="s">
         <v>30</v>
@@ -12050,7 +12050,7 @@
         <v>178</v>
       </c>
       <c r="AM64" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="AN64" t="s">
         <v>381</v>
@@ -12082,17 +12082,17 @@
         <v>848</v>
       </c>
       <c r="I65">
-        <f>LEN(H65)-LEN(SUBSTITUTE(H65, ",", ""))+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K65" t="s">
         <v>999</v>
       </c>
       <c r="L65" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M65" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="O65" t="s">
         <v>931</v>
@@ -12192,7 +12192,7 @@
         <v>1036</v>
       </c>
       <c r="I66">
-        <f>LEN(H66)-LEN(SUBSTITUTE(H66, ",", ""))+1</f>
+        <f t="shared" ref="I66:I129" si="1">LEN(H66)-LEN(SUBSTITUTE(H66, ",", ""))+1</f>
         <v>4</v>
       </c>
       <c r="J66" t="s">
@@ -12202,10 +12202,10 @@
         <v>1087</v>
       </c>
       <c r="L66" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M66" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="O66" t="s">
         <v>971</v>
@@ -12305,7 +12305,7 @@
         <v>977</v>
       </c>
       <c r="I67">
-        <f>LEN(H67)-LEN(SUBSTITUTE(H67, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J67" t="s">
@@ -12315,10 +12315,10 @@
         <v>1008</v>
       </c>
       <c r="L67" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M67" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="O67" t="s">
         <v>954</v>
@@ -12415,20 +12415,20 @@
         <v>886</v>
       </c>
       <c r="H68" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="I68">
-        <f>LEN(H68)-LEN(SUBSTITUTE(H68, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K68" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="L68" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="M68" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="P68" t="s">
         <v>30</v>
@@ -12522,20 +12522,20 @@
         <v>802</v>
       </c>
       <c r="H69" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="I69">
-        <f>LEN(H69)-LEN(SUBSTITUTE(H69, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="K69" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="L69" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M69" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="P69" t="s">
         <v>30</v>
@@ -12629,23 +12629,23 @@
         <v>1046</v>
       </c>
       <c r="H70" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="I70">
-        <f>LEN(H70)-LEN(SUBSTITUTE(H70, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J70" t="s">
         <v>1102</v>
       </c>
       <c r="K70" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="L70" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M70" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="P70" t="s">
         <v>30</v>
@@ -12739,23 +12739,23 @@
         <v>882</v>
       </c>
       <c r="H71" t="s">
+        <v>1195</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J71" t="s">
+        <v>1196</v>
+      </c>
+      <c r="K71" t="s">
         <v>1197</v>
       </c>
-      <c r="I71">
-        <f>LEN(H71)-LEN(SUBSTITUTE(H71, ",", ""))+1</f>
-        <v>4</v>
-      </c>
-      <c r="J71" t="s">
-        <v>1198</v>
-      </c>
-      <c r="K71" t="s">
-        <v>1199</v>
-      </c>
       <c r="L71" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M71" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="P71" t="s">
         <v>30</v>
@@ -12846,26 +12846,26 @@
         <v>855</v>
       </c>
       <c r="G72" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="H72" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="I72">
-        <f>LEN(H72)-LEN(SUBSTITUTE(H72, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J72" t="s">
         <v>1102</v>
       </c>
       <c r="K72" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="L72" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M72" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="P72" t="s">
         <v>30</v>
@@ -12961,20 +12961,20 @@
         <v>788</v>
       </c>
       <c r="H73" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="I73">
-        <f>LEN(H73)-LEN(SUBSTITUTE(H73, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K73" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="L73" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M73" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="P73" t="s">
         <v>30</v>
@@ -13068,23 +13068,23 @@
         <v>865</v>
       </c>
       <c r="H74" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="I74">
-        <f>LEN(H74)-LEN(SUBSTITUTE(H74, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J74" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K74" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="L74" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="M74" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="P74" t="s">
         <v>30</v>
@@ -13181,7 +13181,7 @@
         <v>1123</v>
       </c>
       <c r="I75">
-        <f>LEN(H75)-LEN(SUBSTITUTE(H75, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J75" t="s">
@@ -13191,10 +13191,10 @@
         <v>1118</v>
       </c>
       <c r="L75" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M75" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="P75" t="s">
         <v>30</v>
@@ -13290,23 +13290,23 @@
         <v>802</v>
       </c>
       <c r="H76" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="I76">
-        <f>LEN(H76)-LEN(SUBSTITUTE(H76, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J76" t="s">
         <v>1102</v>
       </c>
       <c r="K76" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="L76" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M76" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="P76" t="s">
         <v>30</v>
@@ -13371,7 +13371,7 @@
         <v>54</v>
       </c>
       <c r="AM76" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="AN76" t="s">
         <v>540</v>
@@ -13394,29 +13394,29 @@
         <v>570</v>
       </c>
       <c r="F77" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="G77" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="H77" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="I77">
-        <f>LEN(H77)-LEN(SUBSTITUTE(H77, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J77" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K77" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="L77" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M77" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="P77" t="s">
         <v>30</v>
@@ -13507,26 +13507,26 @@
         <v>765</v>
       </c>
       <c r="G78" t="s">
+        <v>1172</v>
+      </c>
+      <c r="H78" t="s">
         <v>1173</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J78" t="s">
         <v>1174</v>
       </c>
-      <c r="I78">
-        <f>LEN(H78)-LEN(SUBSTITUTE(H78, ",", ""))+1</f>
-        <v>4</v>
-      </c>
-      <c r="J78" t="s">
-        <v>1175</v>
-      </c>
       <c r="K78" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="L78" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="M78" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="P78" t="s">
         <v>30</v>
@@ -13626,17 +13626,17 @@
         <v>1036</v>
       </c>
       <c r="I79">
-        <f>LEN(H79)-LEN(SUBSTITUTE(H79, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K79" t="s">
         <v>1033</v>
       </c>
       <c r="L79" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M79" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="P79" t="s">
         <v>30</v>
@@ -13733,23 +13733,23 @@
         <v>754</v>
       </c>
       <c r="H80" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="I80">
-        <f>LEN(H80)-LEN(SUBSTITUTE(H80, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J80" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="K80" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="L80" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M80" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="P80" t="s">
         <v>30</v>
@@ -13843,20 +13843,20 @@
         <v>894</v>
       </c>
       <c r="H81" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="I81">
-        <f>LEN(H81)-LEN(SUBSTITUTE(H81, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K81" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="L81" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M81" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="P81" t="s">
         <v>30</v>
@@ -13955,23 +13955,23 @@
         <v>847</v>
       </c>
       <c r="H82" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="I82">
-        <f>LEN(H82)-LEN(SUBSTITUTE(H82, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J82" t="s">
         <v>1102</v>
       </c>
       <c r="K82" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="L82" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M82" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="P82" t="s">
         <v>30</v>
@@ -14070,17 +14070,17 @@
         <v>1025</v>
       </c>
       <c r="I83">
-        <f>LEN(H83)-LEN(SUBSTITUTE(H83, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K83" t="s">
         <v>1032</v>
       </c>
       <c r="L83" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M83" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="P83" t="s">
         <v>30</v>
@@ -14177,10 +14177,10 @@
         <v>1112</v>
       </c>
       <c r="H84" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="I84">
-        <f>LEN(H84)-LEN(SUBSTITUTE(H84, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J84" t="s">
@@ -14190,10 +14190,10 @@
         <v>1116</v>
       </c>
       <c r="L84" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M84" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="P84" t="s">
         <v>30</v>
@@ -14292,7 +14292,7 @@
         <v>1014</v>
       </c>
       <c r="I85">
-        <f>LEN(H85)-LEN(SUBSTITUTE(H85, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J85" t="s">
@@ -14302,10 +14302,10 @@
         <v>1012</v>
       </c>
       <c r="L85" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M85" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="P85" t="s">
         <v>30</v>
@@ -14402,7 +14402,7 @@
         <v>1082</v>
       </c>
       <c r="I86">
-        <f>LEN(H86)-LEN(SUBSTITUTE(H86, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J86" t="s">
@@ -14412,10 +14412,10 @@
         <v>1092</v>
       </c>
       <c r="L86" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M86" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="P86" t="s">
         <v>30</v>
@@ -14512,7 +14512,7 @@
         <v>892</v>
       </c>
       <c r="I87">
-        <f>LEN(H87)-LEN(SUBSTITUTE(H87, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J87" t="s">
@@ -14522,10 +14522,10 @@
         <v>1007</v>
       </c>
       <c r="L87" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="M87" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="O87" t="s">
         <v>948</v>
@@ -14625,7 +14625,7 @@
         <v>892</v>
       </c>
       <c r="I88">
-        <f>LEN(H88)-LEN(SUBSTITUTE(H88, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J88" t="s">
@@ -14635,10 +14635,10 @@
         <v>1039</v>
       </c>
       <c r="L88" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="M88" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="P88" t="s">
         <v>30</v>
@@ -14737,17 +14737,17 @@
         <v>1059</v>
       </c>
       <c r="I89">
-        <f>LEN(H89)-LEN(SUBSTITUTE(H89, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K89" t="s">
         <v>1057</v>
       </c>
       <c r="L89" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="M89" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="O89" t="s">
         <v>968</v>
@@ -14849,7 +14849,7 @@
         <v>1047</v>
       </c>
       <c r="I90">
-        <f>LEN(H90)-LEN(SUBSTITUTE(H90, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J90" t="s">
@@ -14859,10 +14859,10 @@
         <v>1045</v>
       </c>
       <c r="L90" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="M90" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="O90" t="s">
         <v>962</v>
@@ -14962,7 +14962,7 @@
         <v>1085</v>
       </c>
       <c r="I91">
-        <f>LEN(H91)-LEN(SUBSTITUTE(H91, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J91" t="s">
@@ -14972,10 +14972,10 @@
         <v>1093</v>
       </c>
       <c r="L91" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="M91" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="P91" t="s">
         <v>30</v>
@@ -15074,7 +15074,7 @@
         <v>793</v>
       </c>
       <c r="I92">
-        <f>LEN(H92)-LEN(SUBSTITUTE(H92, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J92" t="s">
@@ -15084,10 +15084,10 @@
         <v>992</v>
       </c>
       <c r="L92" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M92" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="N92" t="s">
         <v>795</v>
@@ -15187,17 +15187,17 @@
         <v>755</v>
       </c>
       <c r="H93" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="I93">
-        <f>LEN(H93)-LEN(SUBSTITUTE(H93, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K93" t="s">
         <v>988</v>
       </c>
       <c r="L93" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M93" t="s">
         <v>849</v>
@@ -15299,23 +15299,23 @@
         <v>778</v>
       </c>
       <c r="H94" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="I94">
-        <f>LEN(H94)-LEN(SUBSTITUTE(H94, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J94" t="s">
         <v>1102</v>
       </c>
       <c r="K94" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="L94" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M94" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="P94" t="s">
         <v>30</v>
@@ -15409,23 +15409,23 @@
         <v>842</v>
       </c>
       <c r="H95" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="I95">
-        <f>LEN(H95)-LEN(SUBSTITUTE(H95, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J95" t="s">
         <v>1102</v>
       </c>
       <c r="K95" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="L95" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M95" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="P95" t="s">
         <v>30</v>
@@ -15524,17 +15524,17 @@
         <v>1070</v>
       </c>
       <c r="I96">
-        <f>LEN(H96)-LEN(SUBSTITUTE(H96, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K96" t="s">
         <v>1090</v>
       </c>
       <c r="L96" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M96" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="P96" t="s">
         <v>30</v>
@@ -15599,7 +15599,7 @@
         <v>54</v>
       </c>
       <c r="AM96" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="AN96" t="s">
         <v>386</v>
@@ -15628,23 +15628,23 @@
         <v>1124</v>
       </c>
       <c r="H97" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="I97">
-        <f>LEN(H97)-LEN(SUBSTITUTE(H97, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J97" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="K97" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="L97" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M97" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="P97" t="s">
         <v>30</v>
@@ -15741,17 +15741,17 @@
         <v>797</v>
       </c>
       <c r="I98">
-        <f>LEN(H98)-LEN(SUBSTITUTE(H98, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K98" t="s">
         <v>993</v>
       </c>
       <c r="L98" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="M98" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="O98" t="s">
         <v>912</v>
@@ -15853,7 +15853,7 @@
         <v>1030</v>
       </c>
       <c r="I99">
-        <f>LEN(H99)-LEN(SUBSTITUTE(H99, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J99" t="s">
@@ -15863,10 +15863,10 @@
         <v>1031</v>
       </c>
       <c r="L99" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M99" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="P99" t="s">
         <v>30</v>
@@ -15960,26 +15960,26 @@
         <v>770</v>
       </c>
       <c r="G100" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="H100" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="I100">
-        <f>LEN(H100)-LEN(SUBSTITUTE(H100, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J100" t="s">
         <v>853</v>
       </c>
       <c r="K100" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="L100" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="M100" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="P100" t="s">
         <v>30</v>
@@ -16044,7 +16044,7 @@
         <v>34</v>
       </c>
       <c r="AM100" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="AN100" t="s">
         <v>640</v>
@@ -16067,29 +16067,29 @@
         <v>625</v>
       </c>
       <c r="F101" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="G101" t="s">
         <v>817</v>
       </c>
       <c r="H101" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="I101">
-        <f>LEN(H101)-LEN(SUBSTITUTE(H101, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="J101" t="s">
         <v>1102</v>
       </c>
       <c r="K101" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="L101" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="M101" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="P101" t="s">
         <v>30</v>
@@ -16183,23 +16183,23 @@
         <v>778</v>
       </c>
       <c r="H102" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="I102">
-        <f>LEN(H102)-LEN(SUBSTITUTE(H102, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J102" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="K102" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="L102" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M102" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="P102" t="s">
         <v>30</v>
@@ -16264,7 +16264,7 @@
         <v>44</v>
       </c>
       <c r="AM102" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="AN102" t="s">
         <v>580</v>
@@ -16290,23 +16290,23 @@
         <v>882</v>
       </c>
       <c r="G103" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="H103" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="I103">
-        <f>LEN(H103)-LEN(SUBSTITUTE(H103, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K103" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="L103" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M103" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="P103" t="s">
         <v>30</v>
@@ -16406,17 +16406,17 @@
         <v>800</v>
       </c>
       <c r="I104">
-        <f>LEN(H104)-LEN(SUBSTITUTE(H104, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K104" t="s">
         <v>994</v>
       </c>
       <c r="L104" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="M104" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="O104" t="s">
         <v>914</v>
@@ -16513,23 +16513,23 @@
         <v>841</v>
       </c>
       <c r="H105" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="I105">
-        <f>LEN(H105)-LEN(SUBSTITUTE(H105, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J105" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="K105" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="L105" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M105" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="P105" t="s">
         <v>30</v>
@@ -16623,23 +16623,23 @@
         <v>754</v>
       </c>
       <c r="H106" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="I106">
-        <f>LEN(H106)-LEN(SUBSTITUTE(H106, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J106" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="K106" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="L106" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="M106" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="P106" t="s">
         <v>30</v>
@@ -16736,17 +16736,17 @@
         <v>828</v>
       </c>
       <c r="I107">
-        <f>LEN(H107)-LEN(SUBSTITUTE(H107, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K107" t="s">
         <v>995</v>
       </c>
       <c r="L107" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="M107" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="O107" t="s">
         <v>929</v>
@@ -16843,23 +16843,23 @@
         <v>778</v>
       </c>
       <c r="H108" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
       <c r="I108">
-        <f>LEN(H108)-LEN(SUBSTITUTE(H108, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J108" t="s">
         <v>1102</v>
       </c>
       <c r="K108" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="L108" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="M108" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="P108" t="s">
         <v>30</v>
@@ -16956,23 +16956,23 @@
         <v>852</v>
       </c>
       <c r="I109">
-        <f>LEN(H109)-LEN(SUBSTITUTE(H109, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K109" t="s">
         <v>1000</v>
       </c>
       <c r="L109" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="M109" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="N109" t="s">
         <v>933</v>
       </c>
       <c r="O109" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="P109" t="s">
         <v>30</v>
@@ -17069,17 +17069,17 @@
         <v>1066</v>
       </c>
       <c r="I110">
-        <f>LEN(H110)-LEN(SUBSTITUTE(H110, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K110" t="s">
         <v>1088</v>
       </c>
       <c r="L110" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="M110" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="O110" t="s">
         <v>972</v>
@@ -17176,14 +17176,14 @@
         <v>869</v>
       </c>
       <c r="H111" t="s">
-        <v>1212</v>
+        <v>1210</v>
       </c>
       <c r="I111">
-        <f>LEN(H111)-LEN(SUBSTITUTE(H111, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J111" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="P111" t="s">
         <v>30</v>
@@ -17248,7 +17248,7 @@
         <v>49</v>
       </c>
       <c r="AM111" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="AN111" t="s">
         <v>529</v>
@@ -17277,14 +17277,14 @@
         <v>1060</v>
       </c>
       <c r="H112" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="I112">
-        <f>LEN(H112)-LEN(SUBSTITUTE(H112, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J112" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="P112" t="s">
         <v>30</v>
@@ -17349,7 +17349,7 @@
         <v>34</v>
       </c>
       <c r="AM112" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="AN112" t="s">
         <v>746</v>
@@ -17381,7 +17381,7 @@
         <v>862</v>
       </c>
       <c r="I113">
-        <f>LEN(H113)-LEN(SUBSTITUTE(H113, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J113" t="s">
@@ -17485,7 +17485,7 @@
         <v>895</v>
       </c>
       <c r="I114">
-        <f>LEN(H114)-LEN(SUBSTITUTE(H114, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J114" t="s">
@@ -17560,7 +17560,7 @@
         <v>39</v>
       </c>
       <c r="AM114" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="AN114" t="s">
         <v>263</v>
@@ -17586,13 +17586,13 @@
         <v>882</v>
       </c>
       <c r="G115" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H115" t="s">
         <v>1149</v>
       </c>
-      <c r="H115" t="s">
-        <v>1150</v>
-      </c>
       <c r="I115">
-        <f>LEN(H115)-LEN(SUBSTITUTE(H115, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J115" t="s">
@@ -17693,7 +17693,7 @@
         <v>866</v>
       </c>
       <c r="I116">
-        <f>LEN(H116)-LEN(SUBSTITUTE(H116, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J116" t="s">
@@ -17797,7 +17797,7 @@
         <v>1010</v>
       </c>
       <c r="I117">
-        <f>LEN(H117)-LEN(SUBSTITUTE(H117, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J117" t="s">
@@ -17895,17 +17895,17 @@
         <v>802</v>
       </c>
       <c r="G118" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="H118" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="I118">
-        <f>LEN(H118)-LEN(SUBSTITUTE(H118, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J118" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="P118" t="s">
         <v>30</v>
@@ -18002,7 +18002,7 @@
         <v>1027</v>
       </c>
       <c r="I119">
-        <f>LEN(H119)-LEN(SUBSTITUTE(H119, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J119" t="s">
@@ -18103,7 +18103,7 @@
         <v>777</v>
       </c>
       <c r="I120">
-        <f>LEN(H120)-LEN(SUBSTITUTE(H120, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J120" t="s">
@@ -18212,7 +18212,7 @@
         <v>758</v>
       </c>
       <c r="I121">
-        <f>LEN(H121)-LEN(SUBSTITUTE(H121, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J121" t="s">
@@ -18316,7 +18316,7 @@
         <v>879</v>
       </c>
       <c r="I122">
-        <f>LEN(H122)-LEN(SUBSTITUTE(H122, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J122" t="s">
@@ -18420,7 +18420,7 @@
         <v>861</v>
       </c>
       <c r="I123">
-        <f>LEN(H123)-LEN(SUBSTITUTE(H123, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J123" t="s">
@@ -18495,7 +18495,7 @@
         <v>62</v>
       </c>
       <c r="AM123" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="AN123" t="s">
         <v>205</v>
@@ -18527,7 +18527,7 @@
         <v>875</v>
       </c>
       <c r="I124">
-        <f>LEN(H124)-LEN(SUBSTITUTE(H124, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J124" t="s">
@@ -18631,7 +18631,7 @@
         <v>818</v>
       </c>
       <c r="I125">
-        <f>LEN(H125)-LEN(SUBSTITUTE(H125, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J125" t="s">
@@ -18735,10 +18735,10 @@
         <v>1060</v>
       </c>
       <c r="H126" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="I126">
-        <f>LEN(H126)-LEN(SUBSTITUTE(H126, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J126" t="s">
@@ -18833,13 +18833,13 @@
         <v>882</v>
       </c>
       <c r="G127" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="H127" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="I127">
-        <f>LEN(H127)-LEN(SUBSTITUTE(H127, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J127" t="s">
@@ -18939,17 +18939,17 @@
         <v>984</v>
       </c>
       <c r="H128" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="I128">
-        <f>LEN(H128)-LEN(SUBSTITUTE(H128, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J128" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="N128" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="P128" t="s">
         <v>30</v>
@@ -19040,20 +19040,20 @@
         <v>1124</v>
       </c>
       <c r="G129" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="H129" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="I129">
-        <f>LEN(H129)-LEN(SUBSTITUTE(H129, ",", ""))+1</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J129" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="N129" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="P129" t="s">
         <v>30</v>
@@ -19149,14 +19149,14 @@
         <v>882</v>
       </c>
       <c r="H130" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="I130">
-        <f>LEN(H130)-LEN(SUBSTITUTE(H130, ",", ""))+1</f>
+        <f t="shared" ref="I130:I193" si="2">LEN(H130)-LEN(SUBSTITUTE(H130, ",", ""))+1</f>
         <v>9</v>
       </c>
       <c r="J130" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="P130" t="s">
         <v>30</v>
@@ -19258,7 +19258,7 @@
         <v>1052</v>
       </c>
       <c r="I131">
-        <f>LEN(H131)-LEN(SUBSTITUTE(H131, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J131" t="s">
@@ -19362,7 +19362,7 @@
         <v>891</v>
       </c>
       <c r="I132">
-        <f>LEN(H132)-LEN(SUBSTITUTE(H132, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J132" t="s">
@@ -19466,7 +19466,7 @@
         <v>1080</v>
       </c>
       <c r="I133">
-        <f>LEN(H133)-LEN(SUBSTITUTE(H133, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J133" t="s">
@@ -19564,10 +19564,10 @@
         <v>577</v>
       </c>
       <c r="H134" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="I134">
-        <f>LEN(H134)-LEN(SUBSTITUTE(H134, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J134" t="s">
@@ -19671,7 +19671,7 @@
         <v>973</v>
       </c>
       <c r="I135">
-        <f>LEN(H135)-LEN(SUBSTITUTE(H135, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J135" t="s">
@@ -19766,16 +19766,16 @@
         <v>577</v>
       </c>
       <c r="F136" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="G136" t="s">
         <v>842</v>
       </c>
       <c r="H136" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="I136">
-        <f>LEN(H136)-LEN(SUBSTITUTE(H136, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J136" t="s">
@@ -19876,7 +19876,7 @@
         <v>1016</v>
       </c>
       <c r="I137">
-        <f>LEN(H137)-LEN(SUBSTITUTE(H137, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J137" t="s">
@@ -19977,7 +19977,7 @@
         <v>1101</v>
       </c>
       <c r="I138">
-        <f>LEN(H138)-LEN(SUBSTITUTE(H138, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J138" t="s">
@@ -20060,19 +20060,19 @@
       </c>
       <c r="C139" s="2"/>
       <c r="E139" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="F139" t="s">
         <v>792</v>
       </c>
       <c r="G139" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="H139" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="I139">
-        <f>LEN(H139)-LEN(SUBSTITUTE(H139, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J139" t="s">
@@ -20105,13 +20105,13 @@
         <v>772</v>
       </c>
       <c r="G140" t="s">
+        <v>1145</v>
+      </c>
+      <c r="H140" t="s">
         <v>1146</v>
       </c>
-      <c r="H140" t="s">
-        <v>1147</v>
-      </c>
       <c r="I140">
-        <f>LEN(H140)-LEN(SUBSTITUTE(H140, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J140" t="s">
@@ -20211,17 +20211,17 @@
         <v>755</v>
       </c>
       <c r="H141" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="I141">
-        <f>LEN(H141)-LEN(SUBSTITUTE(H141, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J141" t="s">
         <v>1102</v>
       </c>
       <c r="N141" t="s">
-        <v>1201</v>
+        <v>1199</v>
       </c>
       <c r="P141" t="s">
         <v>30</v>
@@ -20320,10 +20320,10 @@
         <v>1046</v>
       </c>
       <c r="H142" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="I142">
-        <f>LEN(H142)-LEN(SUBSTITUTE(H142, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J142" t="s">
@@ -20421,10 +20421,10 @@
         <v>846</v>
       </c>
       <c r="H143" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="I143">
-        <f>LEN(H143)-LEN(SUBSTITUTE(H143, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J143" t="s">
@@ -20495,7 +20495,7 @@
         <v>34</v>
       </c>
       <c r="AM143" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="AN143" t="s">
         <v>454</v>
@@ -20521,13 +20521,13 @@
         <v>772</v>
       </c>
       <c r="G144" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H144" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="I144">
-        <f>LEN(H144)-LEN(SUBSTITUTE(H144, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J144" t="s">
@@ -20622,13 +20622,13 @@
         <v>1058</v>
       </c>
       <c r="G145" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H145" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="I145">
-        <f>LEN(H145)-LEN(SUBSTITUTE(H145, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J145" t="s">
@@ -20723,13 +20723,13 @@
         <v>1058</v>
       </c>
       <c r="G146" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H146" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="I146">
-        <f>LEN(H146)-LEN(SUBSTITUTE(H146, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J146" t="s">
@@ -20773,13 +20773,13 @@
         <v>846</v>
       </c>
       <c r="G147" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="H147" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="I147">
-        <f>LEN(H147)-LEN(SUBSTITUTE(H147, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J147" t="s">
@@ -20876,13 +20876,13 @@
         <v>775</v>
       </c>
       <c r="G148" t="s">
+        <v>1166</v>
+      </c>
+      <c r="H148" t="s">
         <v>1167</v>
       </c>
-      <c r="H148" t="s">
-        <v>1168</v>
-      </c>
       <c r="I148">
-        <f>LEN(H148)-LEN(SUBSTITUTE(H148, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J148" t="s">
@@ -20983,7 +20983,7 @@
         <v>1107</v>
       </c>
       <c r="I149">
-        <f>LEN(H149)-LEN(SUBSTITUTE(H149, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J149" t="s">
@@ -21078,13 +21078,13 @@
         <v>772</v>
       </c>
       <c r="G150" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H150" t="s">
         <v>1139</v>
       </c>
-      <c r="H150" t="s">
-        <v>1140</v>
-      </c>
       <c r="I150">
-        <f>LEN(H150)-LEN(SUBSTITUTE(H150, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J150" t="s">
@@ -21182,14 +21182,14 @@
         <v>755</v>
       </c>
       <c r="H151" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="I151">
-        <f>LEN(H151)-LEN(SUBSTITUTE(H151, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J151" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="P151" t="s">
         <v>30</v>
@@ -21286,7 +21286,7 @@
         <v>872</v>
       </c>
       <c r="I152">
-        <f>LEN(H152)-LEN(SUBSTITUTE(H152, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J152" t="s">
@@ -21390,7 +21390,7 @@
         <v>810</v>
       </c>
       <c r="I153">
-        <f>LEN(H153)-LEN(SUBSTITUTE(H153, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J153" t="s">
@@ -21494,7 +21494,7 @@
         <v>810</v>
       </c>
       <c r="I154">
-        <f>LEN(H154)-LEN(SUBSTITUTE(H154, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J154" t="s">
@@ -21598,7 +21598,7 @@
         <v>860</v>
       </c>
       <c r="I155">
-        <f>LEN(H155)-LEN(SUBSTITUTE(H155, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J155" t="s">
@@ -21693,20 +21693,20 @@
         <v>747</v>
       </c>
       <c r="F156" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G156" t="s">
         <v>1029</v>
       </c>
       <c r="H156" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="I156">
-        <f>LEN(H156)-LEN(SUBSTITUTE(H156, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J156" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="P156" t="s">
         <v>30</v>
@@ -21803,7 +21803,7 @@
         <v>1061</v>
       </c>
       <c r="I157">
-        <f>LEN(H157)-LEN(SUBSTITUTE(H157, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J157" t="s">
@@ -21907,14 +21907,14 @@
         <v>834</v>
       </c>
       <c r="H158" t="s">
+        <v>1143</v>
+      </c>
+      <c r="I158">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J158" t="s">
         <v>1144</v>
-      </c>
-      <c r="I158">
-        <f>LEN(H158)-LEN(SUBSTITUTE(H158, ",", ""))+1</f>
-        <v>2</v>
-      </c>
-      <c r="J158" t="s">
-        <v>1145</v>
       </c>
       <c r="P158" t="s">
         <v>30</v>
@@ -22008,14 +22008,14 @@
         <v>832</v>
       </c>
       <c r="H159" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="I159">
-        <f>LEN(H159)-LEN(SUBSTITUTE(H159, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J159" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="P159" t="s">
         <v>30</v>
@@ -22112,7 +22112,7 @@
         <v>1055</v>
       </c>
       <c r="I160">
-        <f>LEN(H160)-LEN(SUBSTITUTE(H160, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J160" t="s">
@@ -22219,7 +22219,7 @@
         <v>1055</v>
       </c>
       <c r="I161">
-        <f>LEN(H161)-LEN(SUBSTITUTE(H161, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J161" t="s">
@@ -22323,14 +22323,14 @@
         <v>1029</v>
       </c>
       <c r="H162" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="I162">
-        <f>LEN(H162)-LEN(SUBSTITUTE(H162, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J162" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="P162" t="s">
         <v>30</v>
@@ -22395,7 +22395,7 @@
         <v>44</v>
       </c>
       <c r="AM162" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="AN162" t="s">
         <v>738</v>
@@ -22427,7 +22427,7 @@
         <v>1072</v>
       </c>
       <c r="I163">
-        <f>LEN(H163)-LEN(SUBSTITUTE(H163, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J163" t="s">
@@ -22522,17 +22522,17 @@
         <v>1023</v>
       </c>
       <c r="G164" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="H164" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="I164">
-        <f>LEN(H164)-LEN(SUBSTITUTE(H164, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J164" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P164" t="s">
         <v>30</v>
@@ -22597,7 +22597,7 @@
         <v>34</v>
       </c>
       <c r="AM164" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="AN164" t="s">
         <v>572</v>
@@ -22620,20 +22620,20 @@
         <v>672</v>
       </c>
       <c r="F165" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="G165" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="H165" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="I165">
-        <f>LEN(H165)-LEN(SUBSTITUTE(H165, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J165" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P165" t="s">
         <v>30</v>
@@ -22727,14 +22727,14 @@
         <v>808</v>
       </c>
       <c r="H166" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
       <c r="I166">
-        <f>LEN(H166)-LEN(SUBSTITUTE(H166, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J166" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P166" t="s">
         <v>30</v>
@@ -22802,7 +22802,7 @@
         <v>34</v>
       </c>
       <c r="AM166" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="AN166" t="s">
         <v>686</v>
@@ -22828,17 +22828,17 @@
         <v>775</v>
       </c>
       <c r="G167" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="H167" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="I167">
-        <f>LEN(H167)-LEN(SUBSTITUTE(H167, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J167" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P167" t="s">
         <v>30</v>
@@ -22934,17 +22934,17 @@
         <v>855</v>
       </c>
       <c r="G168" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="H168" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="I168">
-        <f>LEN(H168)-LEN(SUBSTITUTE(H168, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J168" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P168" t="s">
         <v>30</v>
@@ -23009,7 +23009,7 @@
         <v>652</v>
       </c>
       <c r="AM168" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="AN168" t="s">
         <v>694</v>
@@ -23038,14 +23038,14 @@
         <v>755</v>
       </c>
       <c r="H169" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="I169">
-        <f>LEN(H169)-LEN(SUBSTITUTE(H169, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J169" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P169" t="s">
         <v>30</v>
@@ -23110,7 +23110,7 @@
         <v>34</v>
       </c>
       <c r="AM169" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="AN169" t="s">
         <v>671</v>
@@ -23139,17 +23139,17 @@
         <v>1029</v>
       </c>
       <c r="H170" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="I170">
-        <f>LEN(H170)-LEN(SUBSTITUTE(H170, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J170" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="N170" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="P170" t="s">
         <v>30</v>
@@ -23240,17 +23240,17 @@
         <v>792</v>
       </c>
       <c r="G171" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H171" t="s">
+        <v>1191</v>
+      </c>
+      <c r="I171">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J171" t="s">
         <v>1192</v>
-      </c>
-      <c r="H171" t="s">
-        <v>1193</v>
-      </c>
-      <c r="I171">
-        <f>LEN(H171)-LEN(SUBSTITUTE(H171, ",", ""))+1</f>
-        <v>3</v>
-      </c>
-      <c r="J171" t="s">
-        <v>1194</v>
       </c>
       <c r="P171" t="s">
         <v>30</v>
@@ -23346,14 +23346,14 @@
         <v>865</v>
       </c>
       <c r="H172" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="I172">
-        <f>LEN(H172)-LEN(SUBSTITUTE(H172, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J172" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="P172" t="s">
         <v>30</v>
@@ -23450,7 +23450,7 @@
         <v>857</v>
       </c>
       <c r="I173">
-        <f>LEN(H173)-LEN(SUBSTITUTE(H173, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J173" t="s">
@@ -23551,10 +23551,10 @@
         <v>771</v>
       </c>
       <c r="H174" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="I174">
-        <f>LEN(H174)-LEN(SUBSTITUTE(H174, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J174" t="s">
@@ -23657,14 +23657,14 @@
         <v>806</v>
       </c>
       <c r="H175" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="I175">
-        <f>LEN(H175)-LEN(SUBSTITUTE(H175, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J175" t="s">
-        <v>1361</v>
+        <v>1359</v>
       </c>
       <c r="P175" t="s">
         <v>30</v>
@@ -23755,17 +23755,17 @@
         <v>770</v>
       </c>
       <c r="G176" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="H176" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="I176">
-        <f>LEN(H176)-LEN(SUBSTITUTE(H176, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J176" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="P176" t="s">
         <v>30</v>
@@ -23859,14 +23859,14 @@
         <v>865</v>
       </c>
       <c r="H177" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="I177">
-        <f>LEN(H177)-LEN(SUBSTITUTE(H177, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J177" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="P177" t="s">
         <v>30</v>
@@ -23960,14 +23960,14 @@
         <v>788</v>
       </c>
       <c r="H178" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="I178">
-        <f>LEN(H178)-LEN(SUBSTITUTE(H178, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J178" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="P178" t="s">
         <v>30</v>
@@ -24061,10 +24061,10 @@
         <v>839</v>
       </c>
       <c r="H179" t="s">
-        <v>1125</v>
+        <v>1489</v>
       </c>
       <c r="I179">
-        <f>LEN(H179)-LEN(SUBSTITUTE(H179, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J179" t="s">
@@ -24162,13 +24162,13 @@
         <v>1023</v>
       </c>
       <c r="G180" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H180" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="I180">
-        <f>LEN(H180)-LEN(SUBSTITUTE(H180, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J180" t="s">
@@ -24265,13 +24265,13 @@
         <v>802</v>
       </c>
       <c r="G181" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="H181" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="I181">
-        <f>LEN(H181)-LEN(SUBSTITUTE(H181, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J181" t="s">
@@ -24372,7 +24372,7 @@
         <v>844</v>
       </c>
       <c r="I182">
-        <f>LEN(H182)-LEN(SUBSTITUTE(H182, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J182" t="s">
@@ -24473,14 +24473,14 @@
         <v>806</v>
       </c>
       <c r="H183" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="I183">
-        <f>LEN(H183)-LEN(SUBSTITUTE(H183, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J183" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="P183" t="s">
         <v>30</v>
@@ -24545,7 +24545,7 @@
         <v>44</v>
       </c>
       <c r="AM183" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="AN183" t="s">
         <v>635</v>
@@ -24577,7 +24577,7 @@
         <v>974</v>
       </c>
       <c r="I184">
-        <f>LEN(H184)-LEN(SUBSTITUTE(H184, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O184" t="s">
@@ -24675,10 +24675,10 @@
         <v>761</v>
       </c>
       <c r="H185" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="I185">
-        <f>LEN(H185)-LEN(SUBSTITUTE(H185, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O185" t="s">
@@ -24779,7 +24779,7 @@
         <v>1054</v>
       </c>
       <c r="I186">
-        <f>LEN(H186)-LEN(SUBSTITUTE(H186, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O186" t="s">
@@ -24880,7 +24880,7 @@
         <v>982</v>
       </c>
       <c r="I187">
-        <f>LEN(H187)-LEN(SUBSTITUTE(H187, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O187" t="s">
@@ -24984,7 +24984,7 @@
         <v>791</v>
       </c>
       <c r="I188">
-        <f>LEN(H188)-LEN(SUBSTITUTE(H188, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O188" t="s">
@@ -25085,7 +25085,7 @@
         <v>826</v>
       </c>
       <c r="I189">
-        <f>LEN(H189)-LEN(SUBSTITUTE(H189, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O189" t="s">
@@ -25186,7 +25186,7 @@
         <v>804</v>
       </c>
       <c r="I190">
-        <f>LEN(H190)-LEN(SUBSTITUTE(H190, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O190" t="s">
@@ -25290,7 +25290,7 @@
         <v>975</v>
       </c>
       <c r="I191">
-        <f>LEN(H191)-LEN(SUBSTITUTE(H191, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O191" t="s">
@@ -25394,7 +25394,7 @@
         <v>820</v>
       </c>
       <c r="I192">
-        <f>LEN(H192)-LEN(SUBSTITUTE(H192, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O192" t="s">
@@ -25495,7 +25495,7 @@
         <v>787</v>
       </c>
       <c r="I193">
-        <f>LEN(H193)-LEN(SUBSTITUTE(H193, ",", ""))+1</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O193" t="s">
@@ -25598,7 +25598,7 @@
         <v>799</v>
       </c>
       <c r="I194">
-        <f>LEN(H194)-LEN(SUBSTITUTE(H194, ",", ""))+1</f>
+        <f t="shared" ref="I194:I242" si="3">LEN(H194)-LEN(SUBSTITUTE(H194, ",", ""))+1</f>
         <v>3</v>
       </c>
       <c r="O194" t="s">
@@ -25699,7 +25699,7 @@
         <v>801</v>
       </c>
       <c r="I195">
-        <f>LEN(H195)-LEN(SUBSTITUTE(H195, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O195" t="s">
@@ -25800,7 +25800,7 @@
         <v>784</v>
       </c>
       <c r="I196">
-        <f>LEN(H196)-LEN(SUBSTITUTE(H196, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="O196" t="s">
@@ -25901,7 +25901,7 @@
         <v>807</v>
       </c>
       <c r="I197">
-        <f>LEN(H197)-LEN(SUBSTITUTE(H197, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O197" t="s">
@@ -26002,7 +26002,7 @@
         <v>1053</v>
       </c>
       <c r="I198">
-        <f>LEN(H198)-LEN(SUBSTITUTE(H198, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O198" t="s">
@@ -26103,7 +26103,7 @@
         <v>785</v>
       </c>
       <c r="I199">
-        <f>LEN(H199)-LEN(SUBSTITUTE(H199, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="O199" t="s">
@@ -26204,7 +26204,7 @@
         <v>871</v>
       </c>
       <c r="I200">
-        <f>LEN(H200)-LEN(SUBSTITUTE(H200, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O200" t="s">
@@ -26305,7 +26305,7 @@
         <v>1062</v>
       </c>
       <c r="I201">
-        <f>LEN(H201)-LEN(SUBSTITUTE(H201, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O201" t="s">
@@ -26406,7 +26406,7 @@
         <v>821</v>
       </c>
       <c r="I202">
-        <f>LEN(H202)-LEN(SUBSTITUTE(H202, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O202" t="s">
@@ -26507,7 +26507,7 @@
         <v>1041</v>
       </c>
       <c r="I203">
-        <f>LEN(H203)-LEN(SUBSTITUTE(H203, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O203" t="s">
@@ -26608,7 +26608,7 @@
         <v>809</v>
       </c>
       <c r="I204">
-        <f>LEN(H204)-LEN(SUBSTITUTE(H204, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O204" t="s">
@@ -26709,7 +26709,7 @@
         <v>979</v>
       </c>
       <c r="I205">
-        <f>LEN(H205)-LEN(SUBSTITUTE(H205, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="O205" t="s">
@@ -26810,7 +26810,7 @@
         <v>823</v>
       </c>
       <c r="I206">
-        <f>LEN(H206)-LEN(SUBSTITUTE(H206, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="O206" t="s">
@@ -26911,7 +26911,7 @@
         <v>880</v>
       </c>
       <c r="I207">
-        <f>LEN(H207)-LEN(SUBSTITUTE(H207, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="O207" t="s">
@@ -26980,7 +26980,7 @@
         <v>62</v>
       </c>
       <c r="AM207" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="AN207" t="s">
         <v>255</v>
@@ -27012,7 +27012,7 @@
         <v>981</v>
       </c>
       <c r="I208">
-        <f>LEN(H208)-LEN(SUBSTITUTE(H208, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="O208" t="s">
@@ -27113,7 +27113,7 @@
         <v>782</v>
       </c>
       <c r="I209">
-        <f>LEN(H209)-LEN(SUBSTITUTE(H209, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="N209" t="s">
@@ -27214,10 +27214,10 @@
         <v>755</v>
       </c>
       <c r="H210" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="I210">
-        <f>LEN(H210)-LEN(SUBSTITUTE(H210, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P210" t="s">
@@ -27315,7 +27315,7 @@
         <v>1022</v>
       </c>
       <c r="I211">
-        <f>LEN(H211)-LEN(SUBSTITUTE(H211, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P211" t="s">
@@ -27404,16 +27404,16 @@
         <v>628</v>
       </c>
       <c r="F212" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="G212" t="s">
         <v>803</v>
       </c>
       <c r="H212" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="I212">
-        <f>LEN(H212)-LEN(SUBSTITUTE(H212, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P212" t="s">
@@ -27508,14 +27508,14 @@
         <v>803</v>
       </c>
       <c r="H213" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="I213">
-        <f>LEN(H213)-LEN(SUBSTITUTE(H213, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="N213" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="P213" t="s">
         <v>30</v>
@@ -27612,7 +27612,7 @@
         <v>840</v>
       </c>
       <c r="I214">
-        <f>LEN(H214)-LEN(SUBSTITUTE(H214, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P214" t="s">
@@ -27710,7 +27710,7 @@
         <v>880</v>
       </c>
       <c r="I215">
-        <f>LEN(H215)-LEN(SUBSTITUTE(H215, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P215" t="s">
@@ -27811,7 +27811,7 @@
         <v>885</v>
       </c>
       <c r="I216">
-        <f>LEN(H216)-LEN(SUBSTITUTE(H216, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P216" t="s">
@@ -27909,7 +27909,7 @@
         <v>1035</v>
       </c>
       <c r="I217">
-        <f>LEN(H217)-LEN(SUBSTITUTE(H217, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P217" t="s">
@@ -28007,7 +28007,7 @@
         <v>1018</v>
       </c>
       <c r="I218">
-        <f>LEN(H218)-LEN(SUBSTITUTE(H218, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P218" t="s">
@@ -28105,7 +28105,7 @@
         <v>880</v>
       </c>
       <c r="I219">
-        <f>LEN(H219)-LEN(SUBSTITUTE(H219, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P219" t="s">
@@ -28200,10 +28200,10 @@
         <v>766</v>
       </c>
       <c r="H220" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="I220">
-        <f>LEN(H220)-LEN(SUBSTITUTE(H220, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P220" t="s">
@@ -28301,7 +28301,7 @@
         <v>789</v>
       </c>
       <c r="I221">
-        <f>LEN(H221)-LEN(SUBSTITUTE(H221, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P221" t="s">
@@ -28399,7 +28399,7 @@
         <v>790</v>
       </c>
       <c r="I222">
-        <f>LEN(H222)-LEN(SUBSTITUTE(H222, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P222" t="s">
@@ -28491,13 +28491,13 @@
         <v>882</v>
       </c>
       <c r="G223" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="H223" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="I223">
-        <f>LEN(H223)-LEN(SUBSTITUTE(H223, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P223" t="s">
@@ -28594,10 +28594,10 @@
         <v>1048</v>
       </c>
       <c r="H224" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="I224">
-        <f>LEN(H224)-LEN(SUBSTITUTE(H224, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P224" t="s">
@@ -28689,13 +28689,13 @@
         <v>1023</v>
       </c>
       <c r="G225" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="H225" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="I225">
-        <f>LEN(H225)-LEN(SUBSTITUTE(H225, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P225" t="s">
@@ -28793,7 +28793,7 @@
         <v>1028</v>
       </c>
       <c r="I226">
-        <f>LEN(H226)-LEN(SUBSTITUTE(H226, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P226" t="s">
@@ -28882,16 +28882,16 @@
         <v>601</v>
       </c>
       <c r="F227" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="G227" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="H227" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="I227">
-        <f>LEN(H227)-LEN(SUBSTITUTE(H227, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P227" t="s">
@@ -28983,13 +28983,13 @@
         <v>1023</v>
       </c>
       <c r="G228" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="H228" t="s">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="I228">
-        <f>LEN(H228)-LEN(SUBSTITUTE(H228, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P228" t="s">
@@ -29087,7 +29087,7 @@
         <v>835</v>
       </c>
       <c r="I229">
-        <f>LEN(H229)-LEN(SUBSTITUTE(H229, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P229" t="s">
@@ -29187,7 +29187,7 @@
         <v>877</v>
       </c>
       <c r="I230">
-        <f>LEN(H230)-LEN(SUBSTITUTE(H230, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P230" t="s">
@@ -29253,7 +29253,7 @@
         <v>34</v>
       </c>
       <c r="AM230" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="AN230" t="s">
         <v>226</v>
@@ -29282,10 +29282,10 @@
         <v>788</v>
       </c>
       <c r="H231" t="s">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="I231">
-        <f>LEN(H231)-LEN(SUBSTITUTE(H231, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P231" t="s">
@@ -29383,7 +29383,7 @@
         <v>1084</v>
       </c>
       <c r="I232">
-        <f>LEN(H232)-LEN(SUBSTITUTE(H232, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P232" t="s">
@@ -29481,7 +29481,7 @@
         <v>838</v>
       </c>
       <c r="I233">
-        <f>LEN(H233)-LEN(SUBSTITUTE(H233, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P233" t="s">
@@ -29579,10 +29579,10 @@
         <v>802</v>
       </c>
       <c r="H234" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="I234">
-        <f>LEN(H234)-LEN(SUBSTITUTE(H234, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P234" t="s">
@@ -29648,7 +29648,7 @@
         <v>62</v>
       </c>
       <c r="AM234" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="AN234" t="s">
         <v>715</v>
@@ -29674,13 +29674,13 @@
         <v>1023</v>
       </c>
       <c r="G235" t="s">
+        <v>1157</v>
+      </c>
+      <c r="H235" t="s">
         <v>1158</v>
       </c>
-      <c r="H235" t="s">
-        <v>1159</v>
-      </c>
       <c r="I235">
-        <f>LEN(H235)-LEN(SUBSTITUTE(H235, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P235" t="s">
@@ -29774,13 +29774,13 @@
         <v>1067</v>
       </c>
       <c r="G236" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="H236" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="I236">
-        <f>LEN(H236)-LEN(SUBSTITUTE(H236, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P236" t="s">
@@ -29872,13 +29872,13 @@
         <v>841</v>
       </c>
       <c r="G237" t="s">
+        <v>1154</v>
+      </c>
+      <c r="H237" t="s">
         <v>1155</v>
       </c>
-      <c r="H237" t="s">
-        <v>1156</v>
-      </c>
       <c r="I237">
-        <f>LEN(H237)-LEN(SUBSTITUTE(H237, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P237" t="s">
@@ -29978,7 +29978,7 @@
         <v>1038</v>
       </c>
       <c r="I238">
-        <f>LEN(H238)-LEN(SUBSTITUTE(H238, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P238" t="s">
@@ -30070,13 +30070,13 @@
         <v>839</v>
       </c>
       <c r="G239" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="H239" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="I239">
-        <f>LEN(H239)-LEN(SUBSTITUTE(H239, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="P239" t="s">
@@ -30174,7 +30174,7 @@
         <v>836</v>
       </c>
       <c r="I240">
-        <f>LEN(H240)-LEN(SUBSTITUTE(H240, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P240" t="s">
@@ -30272,7 +30272,7 @@
         <v>833</v>
       </c>
       <c r="I241">
-        <f>LEN(H241)-LEN(SUBSTITUTE(H241, ",", ""))+1</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P241" t="s">
@@ -30369,14 +30369,14 @@
         <v>841</v>
       </c>
       <c r="G242" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="H242" t="s">
-        <v>1179</v>
+        <v>1488</v>
       </c>
       <c r="I242">
-        <f>LEN(H242)-LEN(SUBSTITUTE(H242, ",", ""))+1</f>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="P242" t="s">
         <v>30</v>
@@ -30462,7 +30462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81DBE14-E6E9-4DC0-B678-91EC9EF5FD52}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>

</xml_diff>